<commit_message>
Update Premium Customer discounts to 15
</commit_message>
<xml_diff>
--- a/customer/rules.xlsx
+++ b/customer/rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasunranasinghe/Development/Java/RnD/Drools/drools-rules/customer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A3D012-BD36-C947-B800-BCA206110B1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D44706-C939-C743-9E62-E02AA72A8F12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -525,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3">

</xml_diff>

<commit_message>
update package for alm
</commit_message>
<xml_diff>
--- a/customer/rules.xlsx
+++ b/customer/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasunranasinghe/Development/Java/RnD/Drools/drools-rules/customer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kranasingh\Development\RnD\Drools\drools-rules\customer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D44706-C939-C743-9E62-E02AA72A8F12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328E810F-D31F-45BC-AAD1-939DD384B3FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Import</t>
   </si>
   <si>
-    <t>com.kzone.Customer</t>
-  </si>
-  <si>
     <t>RuleTable Discount Calculation</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Premium Customer</t>
   </si>
   <si>
-    <t>com.kzone.drools</t>
-  </si>
-  <si>
     <t>$customer:Customer</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Old Customer</t>
+  </si>
+  <si>
+    <t>com.alm.wiley.controller.Customer</t>
+  </si>
+  <si>
+    <t>com.alm.wiley.controller.drools</t>
   </si>
 </sst>
 </file>
@@ -440,10 +440,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -463,52 +463,52 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>10</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>20</v>

</xml_diff>